<commit_message>
Clean up test data
Remove/update all paths pointing to `/node/xxx`.
</commit_message>
<xml_diff>
--- a/test-data/bread-crumb-data.xlsx
+++ b/test-data/bread-crumb-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/learnb/git/digiplat-qa/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEA4E21-BF0A-8A48-B16C-39F323BBF743}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB5B473-8673-8144-9F30-6203B727C340}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53720" yWindow="3140" windowWidth="28040" windowHeight="17440" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="10340" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_breadcrumbs" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>path</t>
   </si>
@@ -44,54 +44,116 @@
     <t>Article</t>
   </si>
   <si>
+    <t>Blog Post</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>news-events/cancer-currents-blog/2019/vitamin-d-supplement-cancer-prevention</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation/2019-investigators-site</t>
+  </si>
+  <si>
+    <t>Evenet</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation/dfharvard</t>
+  </si>
+  <si>
+    <t>Cancer Center</t>
+  </si>
+  <si>
+    <t>Cancer Research</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation/chanock-stephen</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>news-events/cancer-currents-blog</t>
+  </si>
+  <si>
+    <t>Blog Series</t>
+  </si>
+  <si>
+    <t>espanol/noticias/temas-y-relatos-blog</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>espanol/tipos/seno/investigacion</t>
+  </si>
+  <si>
+    <t>espanol/tipos/seno</t>
+  </si>
+  <si>
+    <t>types/breast</t>
+  </si>
+  <si>
+    <t>Cancer Type Homepage</t>
+  </si>
+  <si>
+    <t>Mini Landing Page</t>
+  </si>
+  <si>
+    <t>espanol/noticias/comunicados-de-prensa/2019</t>
+  </si>
+  <si>
+    <t>about-nci/organization/dcb/division-of-cancer-biology-test</t>
+  </si>
+  <si>
+    <t>types/breast/research</t>
+  </si>
+  <si>
+    <t>about-cancer/coping/feelings/relaxation</t>
+  </si>
+  <si>
+    <t>espanol/cancer/tratamiento/efectos-secundarios/cambios-piel-unas/prurito-pdq</t>
+  </si>
+  <si>
+    <t>PDQ Drug Info</t>
+  </si>
+  <si>
+    <t>PDQ Cancer Info</t>
+  </si>
+  <si>
+    <t>about-cancer/treatment/drugs/bevacizumab</t>
+  </si>
+  <si>
+    <t>types/stomach/patient/stomach-treatment-pdq</t>
+  </si>
+  <si>
+    <t>news-events/press-releases/2019/brca-exchange-test</t>
+  </si>
+  <si>
     <t>Press Release</t>
   </si>
   <si>
-    <t>Blog Post</t>
-  </si>
-  <si>
-    <t>/node/46</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>/espanol/node/46</t>
-  </si>
-  <si>
-    <t>/node/36</t>
-  </si>
-  <si>
-    <t>Cancer Center</t>
-  </si>
-  <si>
-    <t>/node/31</t>
-  </si>
-  <si>
-    <t>/espanol/node/1</t>
-  </si>
-  <si>
-    <t>/about-cancer/coping/feelings/relaxation</t>
-  </si>
-  <si>
-    <t>/espanol/node/6</t>
-  </si>
-  <si>
-    <t>/node/26</t>
+    <t>espanol/noticias/comunicados-de-prensa/2018/leucemia-llc-ibrutinib-estudio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,9 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,26 +499,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E50E58-C20E-6840-B475-2B9A8D9E132C}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="70.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -466,73 +530,73 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
+      <c r="A3" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -540,25 +604,132 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
(#50) Added tests for Breadcrumb
</commit_message>
<xml_diff>
--- a/test-data/bread-crumb-data.xlsx
+++ b/test-data/bread-crumb-data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB5B473-8673-8144-9F30-6203B727C340}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C19D25A-42C1-48F8-B107-E925D5364FEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_breadcrumbs" sheetId="1" r:id="rId1"/>
+    <sheet name="pages_with_no_breadcrumbs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>path</t>
   </si>
@@ -59,9 +60,6 @@
     <t>about-cancer/coping/feelings/relaxation/2019-investigators-site</t>
   </si>
   <si>
-    <t>Evenet</t>
-  </si>
-  <si>
     <t>about-cancer/coping/feelings/relaxation/dfharvard</t>
   </si>
   <si>
@@ -104,9 +102,6 @@
     <t>Mini Landing Page</t>
   </si>
   <si>
-    <t>espanol/noticias/comunicados-de-prensa/2019</t>
-  </si>
-  <si>
     <t>about-nci/organization/dcb/division-of-cancer-biology-test</t>
   </si>
   <si>
@@ -116,9 +111,6 @@
     <t>about-cancer/coping/feelings/relaxation</t>
   </si>
   <si>
-    <t>espanol/cancer/tratamiento/efectos-secundarios/cambios-piel-unas/prurito-pdq</t>
-  </si>
-  <si>
     <t>PDQ Drug Info</t>
   </si>
   <si>
@@ -138,6 +130,102 @@
   </si>
   <si>
     <t>espanol/noticias/comunicados-de-prensa/2018/leucemia-llc-ibrutinib-estudio</t>
+  </si>
+  <si>
+    <t>about-cancer</t>
+  </si>
+  <si>
+    <t>Landing Page</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>linkpath</t>
+  </si>
+  <si>
+    <t>Home,About Cancer,Coping with Cancer</t>
+  </si>
+  <si>
+    <t>/,/about-cancer,/about-cancer/coping</t>
+  </si>
+  <si>
+    <t>Home,About Cancer,Coping with Cancer,Feelings and Cancer</t>
+  </si>
+  <si>
+    <t>/,/about-cancer,/about-cancer/coping,/about-cancer/coping/feelings</t>
+  </si>
+  <si>
+    <t>/,/about-cancer,/about-cancer/coping,/about-cancer/coping/feelings,/about-cancer/coping/feelings/relaxation</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Home,About Cancer</t>
+  </si>
+  <si>
+    <t>/,/about-cancer</t>
+  </si>
+  <si>
+    <t>Home,Cancer Types</t>
+  </si>
+  <si>
+    <t>/,/types,/types/breast</t>
+  </si>
+  <si>
+    <t>Home,Cancer Types,Breast Cancer</t>
+  </si>
+  <si>
+    <t>/,/types</t>
+  </si>
+  <si>
+    <t>Home,News &amp; Events,Cancer Currents Blog</t>
+  </si>
+  <si>
+    <t>/,/news-events,/news-events/cancer-currents-blog</t>
+  </si>
+  <si>
+    <t>Página principal,Tipos de cáncer,Cáncer de seno (mama)</t>
+  </si>
+  <si>
+    <t>/espanol,/espanol/tipos,/espanol/tipos/seno</t>
+  </si>
+  <si>
+    <t>Home,News &amp; Events</t>
+  </si>
+  <si>
+    <t>/,/news-events</t>
+  </si>
+  <si>
+    <t>Página principal,Tipos de cáncer</t>
+  </si>
+  <si>
+    <t>/espanol,/espanol/tipos</t>
+  </si>
+  <si>
+    <t>/espanol,/espanol/noticias</t>
+  </si>
+  <si>
+    <t>Página principal,Noticias</t>
+  </si>
+  <si>
+    <t>Home,About NCI,NCI Organization</t>
+  </si>
+  <si>
+    <t>/,/about-nci,/about-nci/organization</t>
+  </si>
+  <si>
+    <t>Home,About Cancer,Coping with Cancer,Feelings and Cancer,Learning to Relax</t>
+  </si>
+  <si>
+    <t>espanol/tipos/estomago/paciente/tratamiento-estomago-pdq</t>
   </si>
 </sst>
 </file>
@@ -499,19 +587,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E50E58-C20E-6840-B475-2B9A8D9E132C}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D16" sqref="D16:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="70.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="51.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,8 +611,14 @@
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -532,10 +628,16 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -543,8 +645,14 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -554,181 +662,318 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D54F65-9878-4854-8CCD-A6423ADC111E}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.875" customWidth="1"/>
+    <col min="2" max="2" width="24.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>